<commit_message>
update github before continue work
</commit_message>
<xml_diff>
--- a/Comic Book Movies Trivia Questions.xlsx
+++ b/Comic Book Movies Trivia Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HaroldDavidson/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B23D601-EE77-774A-AE7C-13C5E7EE6837}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A9989F-184A-2A48-AB2C-EC9D70F7AF36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="680" windowWidth="28040" windowHeight="17440" xr2:uid="{C2C0F090-CA59-4644-818C-D4689D4A1583}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="285">
   <si>
     <t>Who is Peter Parker bestfriend in Spiderman Homecoming?</t>
   </si>
@@ -339,6 +339,552 @@
   </si>
   <si>
     <t>Empire State University</t>
+  </si>
+  <si>
+    <t>Who is Batman's secret identity?</t>
+  </si>
+  <si>
+    <t>Who is a bat-inspired Superhero who trains himself physically to fight crime?</t>
+  </si>
+  <si>
+    <t>Who is the only villain credited for having "broken the bat"?</t>
+  </si>
+  <si>
+    <t>Who is Batman's most enduring love interest?</t>
+  </si>
+  <si>
+    <t>Who is Gotham City burglar wears a tight, one-piece outfit anf uses a bullwhip for a weapon?</t>
+  </si>
+  <si>
+    <t>Who is a detective that became a trusted Ally to Batman during Bane's reign of terror?</t>
+  </si>
+  <si>
+    <t>Who is the daughter of the Super villain Ra's al Ghul?</t>
+  </si>
+  <si>
+    <t>Who is the expert lawyer and tactician and one of Batman's most enduring enemies?</t>
+  </si>
+  <si>
+    <t>Who is the head of the Ghoul and also called the Chief Demon?</t>
+  </si>
+  <si>
+    <t>Who is the self-proclaimed "Master of Fear" ex-professor of psychology in Gotham City? </t>
+  </si>
+  <si>
+    <t>Who is a powerful, corrupt businessman enemy of Batman?</t>
+  </si>
+  <si>
+    <t>Who id the Executive Vice President of Dagget Industries?</t>
+  </si>
+  <si>
+    <t>Who is the Police Commissionare friend of Batman?</t>
+  </si>
+  <si>
+    <t>Who is a frequent ally and sidekick of Catwoman?</t>
+  </si>
+  <si>
+    <t>Who is the Business Manager at Wayne Enterprises that Batman's equipment needs?</t>
+  </si>
+  <si>
+    <t>Who is a Russian nuclear Physicist that was captured by Bane to create nuclear?</t>
+  </si>
+  <si>
+    <t>Who is special ops Captain who snuck into Gotham City to help fight against bane and his force?</t>
+  </si>
+  <si>
+    <t>Who is a fortysomething police veteran of Gotham City Police Department major Crimes unit?</t>
+  </si>
+  <si>
+    <t>Who is the mayor of Gotham City?</t>
+  </si>
+  <si>
+    <t>What is Bane power that helps him enhanced his stamina</t>
+  </si>
+  <si>
+    <t>Who trained Batman?</t>
+  </si>
+  <si>
+    <t>Who is the deputy Police Cimminssioner in the Gotham City?</t>
+  </si>
+  <si>
+    <t>Who is Bruce Wayne mentor?</t>
+  </si>
+  <si>
+    <t>Who is a board member at Wayne Enterprises?</t>
+  </si>
+  <si>
+    <t>What is a prison anh a genetic modification facility?</t>
+  </si>
+  <si>
+    <t>Bruce Wayne</t>
+  </si>
+  <si>
+    <t>Batman</t>
+  </si>
+  <si>
+    <t>Bane</t>
+  </si>
+  <si>
+    <t>Selina Kyle</t>
+  </si>
+  <si>
+    <t>Catwoman</t>
+  </si>
+  <si>
+    <t>John Blake</t>
+  </si>
+  <si>
+    <t>Talia al Ghul</t>
+  </si>
+  <si>
+    <t>Harvey Dent</t>
+  </si>
+  <si>
+    <t>Ra's al Ghul</t>
+  </si>
+  <si>
+    <t>scarecrow</t>
+  </si>
+  <si>
+    <t>Roland Duaget</t>
+  </si>
+  <si>
+    <t>Philip Stryver</t>
+  </si>
+  <si>
+    <t>James Gordon</t>
+  </si>
+  <si>
+    <t>Holly Robinson</t>
+  </si>
+  <si>
+    <t>Lucius Fox</t>
+  </si>
+  <si>
+    <t>Dr. Pavel</t>
+  </si>
+  <si>
+    <t>Captain Jones</t>
+  </si>
+  <si>
+    <t>Detective Crispus</t>
+  </si>
+  <si>
+    <t>Anthony Garcia</t>
+  </si>
+  <si>
+    <t>Venum</t>
+  </si>
+  <si>
+    <t>Kirigi</t>
+  </si>
+  <si>
+    <t>Hennri Dicard</t>
+  </si>
+  <si>
+    <t>Peter Foley</t>
+  </si>
+  <si>
+    <t>Doughlas Frederick</t>
+  </si>
+  <si>
+    <t>Blackgate Penetentiary</t>
+  </si>
+  <si>
+    <t>Who was replaced as keeper of Bifrost Bridge?</t>
+  </si>
+  <si>
+    <t>Who replaced Heimdall as keeper of the Bifrost Bridge?</t>
+  </si>
+  <si>
+    <t>Who says " I've got this completely under control" in the midst of a battle?</t>
+  </si>
+  <si>
+    <t>Where did the battle happened?</t>
+  </si>
+  <si>
+    <t>Who plays Thor in the movie?</t>
+  </si>
+  <si>
+    <t>What name does Thor and Loki have callef Borr?</t>
+  </si>
+  <si>
+    <t>Who was called " God of Thunder"?</t>
+  </si>
+  <si>
+    <t>Who was impersonating Odin?</t>
+  </si>
+  <si>
+    <t>Who gives advice to Thor that next time they should start with the Big one?</t>
+  </si>
+  <si>
+    <t>What is the name of the only woman and Thor childhood friend?</t>
+  </si>
+  <si>
+    <t>Where do Thor and the rest of his race live?</t>
+  </si>
+  <si>
+    <t>What is called "earth" in one of this Nine Realms of Norse Mythology?</t>
+  </si>
+  <si>
+    <t>How was Hela related to Thor?</t>
+  </si>
+  <si>
+    <t>Who is the former leader of Asgard's Armies?</t>
+  </si>
+  <si>
+    <t>Who attemped to kill Thor?</t>
+  </si>
+  <si>
+    <t>What are the monsters that also known as the Stone Men from Saturn?</t>
+  </si>
+  <si>
+    <t>Which other member of the Avengers did Thor have to fight?</t>
+  </si>
+  <si>
+    <t>Who is the scientist and one of the firsy Earthlings Thor meets after being banish from Asgard?</t>
+  </si>
+  <si>
+    <t>Who utters "That was for New York" after meeting Loki?</t>
+  </si>
+  <si>
+    <t>Who is Thor adoptive brother?</t>
+  </si>
+  <si>
+    <t>What is the name of Thor's hammer?</t>
+  </si>
+  <si>
+    <t>Who helped Thor to locate his missing father?</t>
+  </si>
+  <si>
+    <t>Who says this to Loki" betray him, and I'll kill you"</t>
+  </si>
+  <si>
+    <t>What is the name of Jane's young quirty assistant?</t>
+  </si>
+  <si>
+    <t>Which part ofMalekith's face did Thor manage to scar?</t>
+  </si>
+  <si>
+    <t>What is an ancient Germanic myth that featured dead foeries and huntsmen in pursuit of something in the skies?</t>
+  </si>
+  <si>
+    <t>Who is a more colorful and flamboyant Dark elf?</t>
+  </si>
+  <si>
+    <t>Who took Thor and turned him over to the Grand master to be forced into becoming a fighter?</t>
+  </si>
+  <si>
+    <t>What name Valkyrie was known as?</t>
+  </si>
+  <si>
+    <t>Which character states this dryly? "well done. you just decapitated your grandfather"?</t>
+  </si>
+  <si>
+    <t>Who says " You're big.I've fought bigger"? </t>
+  </si>
+  <si>
+    <t>Who is Thor's friend and not a member of the Warriors Three?</t>
+  </si>
+  <si>
+    <t>What was amicable character poked fun at Loki?</t>
+  </si>
+  <si>
+    <t>Who is the King of Jotunheim?</t>
+  </si>
+  <si>
+    <t>What does Thor ate to recharge his human form?</t>
+  </si>
+  <si>
+    <t>What does they called for Asgardian guard?</t>
+  </si>
+  <si>
+    <t>Who was the fighter trying to start a revolution on Sakaar?</t>
+  </si>
+  <si>
+    <t>Who was an alien made of Rock?</t>
+  </si>
+  <si>
+    <t>Which character is satisfied at someone's fakse narrative?</t>
+  </si>
+  <si>
+    <t>What did Darcy used to Thor when he landed on earth?</t>
+  </si>
+  <si>
+    <t>Where does Thor and Malekith final showdown happened?</t>
+  </si>
+  <si>
+    <t>Which undeground station has Thor found himself when he takes train to greenwich?</t>
+  </si>
+  <si>
+    <t>What object did Thor disguised his hammer as, while on Earth early in the movie?</t>
+  </si>
+  <si>
+    <t>Who curiously asks this "Who's Richard"?</t>
+  </si>
+  <si>
+    <t>Who tells this to Thor" No, there is always hope"?</t>
+  </si>
+  <si>
+    <t>Who is the 'al-seeing, all-hearing guard of the Bifrost bridge in Asgard?</t>
+  </si>
+  <si>
+    <t>Who durects this marvel of a movie?</t>
+  </si>
+  <si>
+    <t>Heimdall</t>
+  </si>
+  <si>
+    <t>Skurge</t>
+  </si>
+  <si>
+    <t>Sif</t>
+  </si>
+  <si>
+    <t>Vanaheim</t>
+  </si>
+  <si>
+    <t>Chris Hemsworth</t>
+  </si>
+  <si>
+    <t>Grandfather</t>
+  </si>
+  <si>
+    <t>Thor</t>
+  </si>
+  <si>
+    <t>Loki</t>
+  </si>
+  <si>
+    <t>Fandral</t>
+  </si>
+  <si>
+    <t>Asgard</t>
+  </si>
+  <si>
+    <t>Midgard</t>
+  </si>
+  <si>
+    <t>Sister</t>
+  </si>
+  <si>
+    <t>Hela</t>
+  </si>
+  <si>
+    <t>Frosy Giants</t>
+  </si>
+  <si>
+    <t>Kronans</t>
+  </si>
+  <si>
+    <t>Hulk</t>
+  </si>
+  <si>
+    <t>Jane Foster</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Mjollnir</t>
+  </si>
+  <si>
+    <t>Dr. Strange</t>
+  </si>
+  <si>
+    <t>Darcy</t>
+  </si>
+  <si>
+    <t>whole right half</t>
+  </si>
+  <si>
+    <t>Wild hunt</t>
+  </si>
+  <si>
+    <t>Malekith</t>
+  </si>
+  <si>
+    <t>Valkyrie</t>
+  </si>
+  <si>
+    <t>Scrapper 142</t>
+  </si>
+  <si>
+    <t>King Laufey</t>
+  </si>
+  <si>
+    <t>pop tarts</t>
+  </si>
+  <si>
+    <t>Einherjar</t>
+  </si>
+  <si>
+    <t>korg</t>
+  </si>
+  <si>
+    <t>Korg</t>
+  </si>
+  <si>
+    <t>Tasers</t>
+  </si>
+  <si>
+    <t>Greenwich</t>
+  </si>
+  <si>
+    <t>Charing cross</t>
+  </si>
+  <si>
+    <t>Umbrella</t>
+  </si>
+  <si>
+    <t>Heimdall </t>
+  </si>
+  <si>
+    <t>Kenneth Branagh</t>
+  </si>
+  <si>
+    <t>Who is a Caped Crusader, the Dark Knight, and the world's greatest Detective?</t>
+  </si>
+  <si>
+    <t>What is Superman baby's name?</t>
+  </si>
+  <si>
+    <t>What is Superman Real name?</t>
+  </si>
+  <si>
+    <t>Who is Superman's love interest?</t>
+  </si>
+  <si>
+    <t>Who is Superman classic Archenemy?</t>
+  </si>
+  <si>
+    <t>Who is Batman's real identity?</t>
+  </si>
+  <si>
+    <t>Who has an official title "Princess Diana of Themyscira, Daughter of Hippolyta"?</t>
+  </si>
+  <si>
+    <t>Who is the King of Atlantis?</t>
+  </si>
+  <si>
+    <t>Who is the deadliest foe of Superman?</t>
+  </si>
+  <si>
+    <t>Who has the power to manipulate electricity, body vibration to phase through objects?</t>
+  </si>
+  <si>
+    <t>Who is a kryptonian greatest and personal enemy of Superman?</t>
+  </si>
+  <si>
+    <t>Who is half human, half machine and a true superhero for modern age?</t>
+  </si>
+  <si>
+    <t>Who has cybernatically enhanced strength and was an adversary of Batman?</t>
+  </si>
+  <si>
+    <t>Who is the mother of Batman and wife of Dr. Thomas Wayne?</t>
+  </si>
+  <si>
+    <t>Who is Batman's loyal bestfriend and has been called "Batman's batman"?</t>
+  </si>
+  <si>
+    <t>Who is the father of Bruce Wayne, and husband of Martha Wayne?</t>
+  </si>
+  <si>
+    <t>Who is the Personal assistant and bodyguard of Lex Luthor?</t>
+  </si>
+  <si>
+    <t>Who is a young photo journalist working for the Daily Planet and a close friend of Superman?</t>
+  </si>
+  <si>
+    <t>Who is a junior Senator that leads hearings to investigate an incident with Superman in Nairomi?</t>
+  </si>
+  <si>
+    <t>Who is the adoptive mother of Clark Kent?</t>
+  </si>
+  <si>
+    <t>Who is a former Wayne Enterprise employee who lost both of his legs as a result if injuries sustained during the Battle of Metropolis?</t>
+  </si>
+  <si>
+    <t>Who is the editor-in-chief of the Metropolis Newspaper the Daily Planet?</t>
+  </si>
+  <si>
+    <t>Who is the adoptive father of Clark Kent?</t>
+  </si>
+  <si>
+    <t>Who won the fight between Superman and Batman?</t>
+  </si>
+  <si>
+    <t>What ability did Batman used against Superman?</t>
+  </si>
+  <si>
+    <t>Kal-El</t>
+  </si>
+  <si>
+    <t>Clark Kent</t>
+  </si>
+  <si>
+    <t>Lois Lane</t>
+  </si>
+  <si>
+    <t>Lex Luthor</t>
+  </si>
+  <si>
+    <t>Wonder Woman</t>
+  </si>
+  <si>
+    <t>Aquaman</t>
+  </si>
+  <si>
+    <t>Doomsday</t>
+  </si>
+  <si>
+    <t>Flash</t>
+  </si>
+  <si>
+    <t>General Zod</t>
+  </si>
+  <si>
+    <t>Cyborg</t>
+  </si>
+  <si>
+    <t>KGBeast</t>
+  </si>
+  <si>
+    <t>Martha Wayne</t>
+  </si>
+  <si>
+    <t>Alfred Pennyworth</t>
+  </si>
+  <si>
+    <t>Thomas Wayne</t>
+  </si>
+  <si>
+    <t>Mercy Graves</t>
+  </si>
+  <si>
+    <t>Jimmy Olsen</t>
+  </si>
+  <si>
+    <t>June Finch</t>
+  </si>
+  <si>
+    <t>Martha Kent</t>
+  </si>
+  <si>
+    <t>Wallace Keefe</t>
+  </si>
+  <si>
+    <t>Perry White</t>
+  </si>
+  <si>
+    <t>Jonathan Kent</t>
+  </si>
+  <si>
+    <t>Superman</t>
+  </si>
+  <si>
+    <t>Kryptonite</t>
   </si>
 </sst>
 </file>
@@ -697,16 +1243,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3815C0A2-2744-B448-9808-A90F13837372}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="B301" sqref="B301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="105.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1274,9 +1821,1831 @@
       <c r="A52" t="s">
         <v>52</v>
       </c>
+      <c r="B52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>52</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>52</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>52</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>52</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>52</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>52</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>52</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>52</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>52</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>52</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>52</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>52</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>52</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>52</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>52</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>52</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>52</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>52</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>52</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>52</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>52</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>52</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>52</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>52</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>52</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>52</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>52</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>52</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>52</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>52</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>52</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>52</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>52</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>52</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>52</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>52</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>52</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>52</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>52</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>52</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>52</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>52</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>52</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>52</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>52</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>52</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>52</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>52</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>52</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>52</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>52</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>52</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>52</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>52</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>52</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>52</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>52</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>52</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>52</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>52</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>52</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>52</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>52</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>52</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>52</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>52</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>52</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>52</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>52</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>52</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>52</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>52</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>52</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>52</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>52</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>52</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>52</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>52</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>52</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>52</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>52</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>52</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>52</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>52</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A291" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A295" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A296" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A297" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A298" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A300" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A301" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>